<commit_message>
add args[2] = endRow
</commit_message>
<xml_diff>
--- a/ConsoleApp2/bin/Debug/netcoreapp3.1/Data/FlextimeSheetForm20200601.xlsx
+++ b/ConsoleApp2/bin/Debug/netcoreapp3.1/Data/FlextimeSheetForm20200601.xlsx
@@ -35,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="23" uniqueCount="23">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="47" uniqueCount="47">
   <si>
     <t>タイムシート</t>
   </si>
@@ -44,6 +44,9 @@
   </si>
   <si>
     <t>氏名：</t>
+  </si>
+  <si>
+    <t>Akiyama</t>
   </si>
   <si>
     <t>日付</t>
@@ -73,7 +76,76 @@
     <t>備考</t>
   </si>
   <si>
+    <t>10:00</t>
+  </si>
+  <si>
+    <t>19:00</t>
+  </si>
+  <si>
+    <t>01:00</t>
+  </si>
+  <si>
+    <t>08:30</t>
+  </si>
+  <si>
+    <t>09:00</t>
+  </si>
+  <si>
+    <t>19:45</t>
+  </si>
+  <si>
+    <t>02:45</t>
+  </si>
+  <si>
+    <t>09:30</t>
+  </si>
+  <si>
+    <t>20:00</t>
+  </si>
+  <si>
+    <t>01:30</t>
+  </si>
+  <si>
     <t xml:space="preserve"> </t>
+  </si>
+  <si>
+    <t>08:00</t>
+  </si>
+  <si>
+    <t>18:45</t>
+  </si>
+  <si>
+    <t>09:40</t>
+  </si>
+  <si>
+    <t>19:30</t>
+  </si>
+  <si>
+    <t>09:45</t>
+  </si>
+  <si>
+    <t>18:30</t>
+  </si>
+  <si>
+    <t>09:15</t>
+  </si>
+  <si>
+    <t>02:00</t>
+  </si>
+  <si>
+    <t>01:15</t>
+  </si>
+  <si>
+    <t>08:45</t>
+  </si>
+  <si>
+    <t>18:00</t>
+  </si>
+  <si>
+    <t>16:30</t>
+  </si>
+  <si>
+    <t>18:15</t>
   </si>
   <si>
     <t>22</t>
@@ -154,7 +226,7 @@
     <numFmt numFmtId="173" formatCode="[h]:mm"/>
     <numFmt numFmtId="174" formatCode="[h]:mm;[Red]\-[h]:mm"/>
   </numFmts>
-  <fonts count="15">
+  <fonts count="16">
     <font>
       <sz val="11"/>
       <name val="ＭＳ Ｐゴシック"/>
@@ -244,6 +316,13 @@
       <name val="Arial"/>
       <family val="2"/>
     </font>
+    <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="ＭＳ Ｐゴシック"/>
+      <family val="3"/>
+      <charset val="128"/>
+    </font>
   </fonts>
   <fills count="3">
     <fill>
@@ -259,7 +338,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="21">
+  <borders count="22">
     <border>
       <left/>
       <right/>
@@ -517,6 +596,19 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0">
@@ -526,7 +618,7 @@
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="80">
+  <cellXfs count="84">
     <xf numFmtId="0" applyNumberFormat="1" fontId="0" applyFont="1" fillId="0" applyFill="1" borderId="0" applyBorder="1" xfId="0" applyProtection="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
@@ -771,6 +863,18 @@
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="20" applyNumberFormat="1" fontId="3" applyFont="1" fillId="0" applyFill="1" borderId="8" applyBorder="1" xfId="0" applyProtection="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" applyNumberFormat="1" fontId="15" applyFont="1" fillId="0" applyFill="1" borderId="2" applyBorder="1" xfId="0" applyProtection="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="20" applyNumberFormat="1" fontId="15" applyFont="1" fillId="0" applyFill="1" borderId="10" applyBorder="1" xfId="0" applyProtection="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="20" applyNumberFormat="1" fontId="15" applyFont="1" fillId="0" applyFill="1" borderId="5" applyBorder="1" xfId="0" applyProtection="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="20" applyNumberFormat="1" fontId="15" applyFont="1" fillId="0" applyFill="1" borderId="21" applyBorder="1" xfId="0" applyProtection="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
@@ -1978,7 +2082,9 @@
       <c r="B5" s="7" t="s">
         <v>2</v>
       </c>
-      <c r="C5" s="55"/>
+      <c r="C5" s="80" t="s">
+        <v>3</v>
+      </c>
       <c r="D5" s="55"/>
       <c r="E5" s="55"/>
       <c r="F5" s="55"/>
@@ -2006,39 +2112,39 @@
     </row>
     <row r="7" ht="16.5" customHeight="1">
       <c r="B7" s="11" t="s">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="C7" s="11" t="s">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="D7" s="56" t="s">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="E7" s="57"/>
       <c r="F7" s="58"/>
       <c r="G7" s="56" t="s">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="H7" s="57"/>
       <c r="I7" s="58"/>
       <c r="J7" s="56" t="s">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="K7" s="57"/>
       <c r="L7" s="58"/>
       <c r="M7" s="56" t="s">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="N7" s="57"/>
       <c r="O7" s="58"/>
       <c r="P7" s="35" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="Q7" s="35" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="R7" s="12" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="S7" s="13"/>
     </row>
@@ -2051,18 +2157,18 @@
         <f ref="C8:C37" t="shared" si="0">WEEKDAY(B8)</f>
         <v>2</v>
       </c>
-      <c r="D8" s="59">
-        <v>0</v>
+      <c r="D8" s="81" t="s">
+        <v>13</v>
       </c>
       <c r="E8" s="60"/>
       <c r="F8" s="61"/>
-      <c r="G8" s="59">
-        <v>0</v>
+      <c r="G8" s="81" t="s">
+        <v>14</v>
       </c>
       <c r="H8" s="60"/>
       <c r="I8" s="61"/>
-      <c r="J8" s="59">
-        <v>0</v>
+      <c r="J8" s="81" t="s">
+        <v>15</v>
       </c>
       <c r="K8" s="60"/>
       <c r="L8" s="61"/>
@@ -2087,18 +2193,18 @@
         <f t="shared" si="0"/>
         <v>3</v>
       </c>
-      <c r="D9" s="59">
-        <v>0</v>
+      <c r="D9" s="82" t="s">
+        <v>16</v>
       </c>
       <c r="E9" s="60"/>
       <c r="F9" s="61"/>
-      <c r="G9" s="59">
-        <v>0</v>
+      <c r="G9" s="82" t="s">
+        <v>14</v>
       </c>
       <c r="H9" s="60"/>
       <c r="I9" s="61"/>
-      <c r="J9" s="59">
-        <v>0</v>
+      <c r="J9" s="82" t="s">
+        <v>15</v>
       </c>
       <c r="K9" s="60"/>
       <c r="L9" s="61"/>
@@ -2123,18 +2229,18 @@
         <f t="shared" si="0"/>
         <v>4</v>
       </c>
-      <c r="D10" s="59">
-        <v>0</v>
+      <c r="D10" s="82" t="s">
+        <v>17</v>
       </c>
       <c r="E10" s="60"/>
       <c r="F10" s="61"/>
-      <c r="G10" s="59">
-        <v>0</v>
+      <c r="G10" s="82" t="s">
+        <v>18</v>
       </c>
       <c r="H10" s="60"/>
       <c r="I10" s="61"/>
-      <c r="J10" s="59">
-        <v>0</v>
+      <c r="J10" s="82" t="s">
+        <v>19</v>
       </c>
       <c r="K10" s="60"/>
       <c r="L10" s="61"/>
@@ -2159,18 +2265,18 @@
         <f t="shared" si="0"/>
         <v>5</v>
       </c>
-      <c r="D11" s="59">
-        <v>0</v>
+      <c r="D11" s="82" t="s">
+        <v>20</v>
       </c>
       <c r="E11" s="60"/>
       <c r="F11" s="61"/>
-      <c r="G11" s="59">
-        <v>0</v>
+      <c r="G11" s="82" t="s">
+        <v>21</v>
       </c>
       <c r="H11" s="60"/>
       <c r="I11" s="61"/>
-      <c r="J11" s="59">
-        <v>0</v>
+      <c r="J11" s="82" t="s">
+        <v>22</v>
       </c>
       <c r="K11" s="60"/>
       <c r="L11" s="61"/>
@@ -2181,10 +2287,10 @@
       <c r="N11" s="60"/>
       <c r="O11" s="61"/>
       <c r="P11" s="48" t="s">
-        <v>12</v>
+        <v>23</v>
       </c>
       <c r="Q11" s="48" t="s">
-        <v>12</v>
+        <v>23</v>
       </c>
       <c r="R11" s="20"/>
       <c r="S11" s="16"/>
@@ -2199,18 +2305,18 @@
         <f t="shared" si="0"/>
         <v>6</v>
       </c>
-      <c r="D12" s="59">
-        <v>0</v>
+      <c r="D12" s="82" t="s">
+        <v>20</v>
       </c>
       <c r="E12" s="60"/>
       <c r="F12" s="61"/>
-      <c r="G12" s="59">
-        <v>0</v>
+      <c r="G12" s="82" t="s">
+        <v>14</v>
       </c>
       <c r="H12" s="60"/>
       <c r="I12" s="61"/>
-      <c r="J12" s="59">
-        <v>0</v>
+      <c r="J12" s="82" t="s">
+        <v>22</v>
       </c>
       <c r="K12" s="60"/>
       <c r="L12" s="61"/>
@@ -2235,23 +2341,17 @@
         <f t="shared" si="0"/>
         <v>7</v>
       </c>
-      <c r="D13" s="59" t="s">
-        <v>12</v>
-      </c>
+      <c r="D13" s="82"/>
       <c r="E13" s="60"/>
       <c r="F13" s="61"/>
-      <c r="G13" s="59" t="s">
-        <v>12</v>
-      </c>
+      <c r="G13" s="82"/>
       <c r="H13" s="60"/>
       <c r="I13" s="61"/>
-      <c r="J13" s="59" t="s">
-        <v>12</v>
-      </c>
+      <c r="J13" s="82"/>
       <c r="K13" s="60"/>
       <c r="L13" s="61"/>
       <c r="M13" s="59" t="s">
-        <v>12</v>
+        <v>23</v>
       </c>
       <c r="N13" s="60"/>
       <c r="O13" s="61"/>
@@ -2270,23 +2370,17 @@
         <f t="shared" si="0"/>
         <v>1</v>
       </c>
-      <c r="D14" s="59" t="s">
-        <v>12</v>
-      </c>
+      <c r="D14" s="82"/>
       <c r="E14" s="60"/>
       <c r="F14" s="61"/>
-      <c r="G14" s="59" t="s">
-        <v>12</v>
-      </c>
+      <c r="G14" s="82"/>
       <c r="H14" s="60"/>
       <c r="I14" s="61"/>
-      <c r="J14" s="59" t="s">
-        <v>12</v>
-      </c>
+      <c r="J14" s="82"/>
       <c r="K14" s="60"/>
       <c r="L14" s="61"/>
       <c r="M14" s="59" t="s">
-        <v>12</v>
+        <v>23</v>
       </c>
       <c r="N14" s="60"/>
       <c r="O14" s="61"/>
@@ -2305,18 +2399,18 @@
         <f t="shared" si="0"/>
         <v>2</v>
       </c>
-      <c r="D15" s="59">
-        <v>0</v>
+      <c r="D15" s="82" t="s">
+        <v>24</v>
       </c>
       <c r="E15" s="60"/>
       <c r="F15" s="61"/>
-      <c r="G15" s="59">
-        <v>0</v>
+      <c r="G15" s="82" t="s">
+        <v>25</v>
       </c>
       <c r="H15" s="60"/>
       <c r="I15" s="61"/>
-      <c r="J15" s="59">
-        <v>0</v>
+      <c r="J15" s="82" t="s">
+        <v>15</v>
       </c>
       <c r="K15" s="60"/>
       <c r="L15" s="61"/>
@@ -2341,18 +2435,18 @@
         <f t="shared" si="0"/>
         <v>3</v>
       </c>
-      <c r="D16" s="59">
-        <v>0</v>
+      <c r="D16" s="82" t="s">
+        <v>24</v>
       </c>
       <c r="E16" s="60"/>
       <c r="F16" s="61"/>
-      <c r="G16" s="59">
-        <v>0</v>
+      <c r="G16" s="82" t="s">
+        <v>14</v>
       </c>
       <c r="H16" s="60"/>
       <c r="I16" s="61"/>
-      <c r="J16" s="59">
-        <v>0</v>
+      <c r="J16" s="82" t="s">
+        <v>15</v>
       </c>
       <c r="K16" s="60"/>
       <c r="L16" s="61"/>
@@ -2377,18 +2471,18 @@
         <f t="shared" si="0"/>
         <v>4</v>
       </c>
-      <c r="D17" s="59">
-        <v>0</v>
+      <c r="D17" s="82" t="s">
+        <v>26</v>
       </c>
       <c r="E17" s="60"/>
       <c r="F17" s="61"/>
-      <c r="G17" s="59">
-        <v>0</v>
+      <c r="G17" s="82" t="s">
+        <v>14</v>
       </c>
       <c r="H17" s="60"/>
       <c r="I17" s="61"/>
-      <c r="J17" s="59">
-        <v>0</v>
+      <c r="J17" s="82" t="s">
+        <v>22</v>
       </c>
       <c r="K17" s="60"/>
       <c r="L17" s="61"/>
@@ -2399,7 +2493,7 @@
       <c r="N17" s="60"/>
       <c r="O17" s="61"/>
       <c r="P17" s="48" t="s">
-        <v>12</v>
+        <v>23</v>
       </c>
       <c r="Q17" s="48"/>
       <c r="R17" s="20"/>
@@ -2415,18 +2509,18 @@
         <f t="shared" si="0"/>
         <v>5</v>
       </c>
-      <c r="D18" s="59">
-        <v>0</v>
+      <c r="D18" s="82" t="s">
+        <v>13</v>
       </c>
       <c r="E18" s="60"/>
       <c r="F18" s="61"/>
-      <c r="G18" s="59">
-        <v>0</v>
+      <c r="G18" s="82" t="s">
+        <v>27</v>
       </c>
       <c r="H18" s="60"/>
       <c r="I18" s="61"/>
-      <c r="J18" s="59">
-        <v>0</v>
+      <c r="J18" s="82" t="s">
+        <v>15</v>
       </c>
       <c r="K18" s="60"/>
       <c r="L18" s="61"/>
@@ -2437,7 +2531,7 @@
       <c r="N18" s="60"/>
       <c r="O18" s="61"/>
       <c r="P18" s="48" t="s">
-        <v>12</v>
+        <v>23</v>
       </c>
       <c r="Q18" s="48"/>
       <c r="R18" s="38"/>
@@ -2453,18 +2547,18 @@
         <f t="shared" si="0"/>
         <v>6</v>
       </c>
-      <c r="D19" s="59">
-        <v>0</v>
+      <c r="D19" s="82" t="s">
+        <v>28</v>
       </c>
       <c r="E19" s="60"/>
       <c r="F19" s="61"/>
-      <c r="G19" s="59">
-        <v>0</v>
+      <c r="G19" s="82" t="s">
+        <v>29</v>
       </c>
       <c r="H19" s="60"/>
       <c r="I19" s="61"/>
-      <c r="J19" s="59">
-        <v>0</v>
+      <c r="J19" s="82" t="s">
+        <v>15</v>
       </c>
       <c r="K19" s="60"/>
       <c r="L19" s="61"/>
@@ -2475,10 +2569,10 @@
       <c r="N19" s="60"/>
       <c r="O19" s="61"/>
       <c r="P19" s="48" t="s">
-        <v>12</v>
+        <v>23</v>
       </c>
       <c r="Q19" s="48" t="s">
-        <v>12</v>
+        <v>23</v>
       </c>
       <c r="R19" s="38"/>
       <c r="S19" s="16"/>
@@ -2493,23 +2587,17 @@
         <f t="shared" si="0"/>
         <v>7</v>
       </c>
-      <c r="D20" s="59" t="s">
-        <v>12</v>
-      </c>
+      <c r="D20" s="82"/>
       <c r="E20" s="60"/>
       <c r="F20" s="61"/>
-      <c r="G20" s="59" t="s">
-        <v>12</v>
-      </c>
+      <c r="G20" s="82"/>
       <c r="H20" s="60"/>
       <c r="I20" s="61"/>
-      <c r="J20" s="59" t="s">
-        <v>12</v>
-      </c>
+      <c r="J20" s="82"/>
       <c r="K20" s="60"/>
       <c r="L20" s="61"/>
       <c r="M20" s="59" t="s">
-        <v>12</v>
+        <v>23</v>
       </c>
       <c r="N20" s="60"/>
       <c r="O20" s="61"/>
@@ -2528,30 +2616,24 @@
         <f t="shared" si="0"/>
         <v>1</v>
       </c>
-      <c r="D21" s="59" t="s">
-        <v>12</v>
-      </c>
+      <c r="D21" s="82"/>
       <c r="E21" s="60"/>
       <c r="F21" s="61"/>
-      <c r="G21" s="59" t="s">
-        <v>12</v>
-      </c>
+      <c r="G21" s="82"/>
       <c r="H21" s="60"/>
       <c r="I21" s="61"/>
-      <c r="J21" s="59" t="s">
-        <v>12</v>
-      </c>
+      <c r="J21" s="82"/>
       <c r="K21" s="60"/>
       <c r="L21" s="61"/>
       <c r="M21" s="59" t="s">
-        <v>12</v>
+        <v>23</v>
       </c>
       <c r="N21" s="60"/>
       <c r="O21" s="61"/>
       <c r="P21" s="48"/>
       <c r="Q21" s="48"/>
       <c r="R21" s="38" t="s">
-        <v>12</v>
+        <v>23</v>
       </c>
       <c r="S21" s="16"/>
       <c r="T21" s="17"/>
@@ -2565,18 +2647,18 @@
         <f t="shared" si="0"/>
         <v>2</v>
       </c>
-      <c r="D22" s="59">
-        <v>0</v>
+      <c r="D22" s="82" t="s">
+        <v>30</v>
       </c>
       <c r="E22" s="60"/>
       <c r="F22" s="61"/>
-      <c r="G22" s="59">
-        <v>0</v>
+      <c r="G22" s="82" t="s">
+        <v>14</v>
       </c>
       <c r="H22" s="60"/>
       <c r="I22" s="61"/>
-      <c r="J22" s="59">
-        <v>0</v>
+      <c r="J22" s="82" t="s">
+        <v>31</v>
       </c>
       <c r="K22" s="60"/>
       <c r="L22" s="61"/>
@@ -2601,18 +2683,18 @@
         <f t="shared" si="0"/>
         <v>3</v>
       </c>
-      <c r="D23" s="59">
-        <v>0</v>
+      <c r="D23" s="82" t="s">
+        <v>28</v>
       </c>
       <c r="E23" s="60"/>
       <c r="F23" s="61"/>
-      <c r="G23" s="59">
-        <v>0</v>
+      <c r="G23" s="82" t="s">
+        <v>14</v>
       </c>
       <c r="H23" s="60"/>
       <c r="I23" s="61"/>
-      <c r="J23" s="59">
-        <v>0</v>
+      <c r="J23" s="82" t="s">
+        <v>32</v>
       </c>
       <c r="K23" s="60"/>
       <c r="L23" s="61"/>
@@ -2637,18 +2719,18 @@
         <f t="shared" si="0"/>
         <v>4</v>
       </c>
-      <c r="D24" s="59">
-        <v>0</v>
+      <c r="D24" s="82" t="s">
+        <v>33</v>
       </c>
       <c r="E24" s="60"/>
       <c r="F24" s="61"/>
-      <c r="G24" s="59">
-        <v>0</v>
+      <c r="G24" s="82" t="s">
+        <v>14</v>
       </c>
       <c r="H24" s="60"/>
       <c r="I24" s="61"/>
-      <c r="J24" s="59">
-        <v>0</v>
+      <c r="J24" s="82" t="s">
+        <v>22</v>
       </c>
       <c r="K24" s="60"/>
       <c r="L24" s="61"/>
@@ -2673,18 +2755,18 @@
         <f t="shared" si="0"/>
         <v>5</v>
       </c>
-      <c r="D25" s="59">
-        <v>0</v>
+      <c r="D25" s="82" t="s">
+        <v>13</v>
       </c>
       <c r="E25" s="60"/>
       <c r="F25" s="61"/>
-      <c r="G25" s="59">
-        <v>0</v>
+      <c r="G25" s="82" t="s">
+        <v>29</v>
       </c>
       <c r="H25" s="60"/>
       <c r="I25" s="61"/>
-      <c r="J25" s="59">
-        <v>0</v>
+      <c r="J25" s="82" t="s">
+        <v>22</v>
       </c>
       <c r="K25" s="60"/>
       <c r="L25" s="61"/>
@@ -2695,7 +2777,7 @@
       <c r="N25" s="60"/>
       <c r="O25" s="61"/>
       <c r="P25" s="48" t="s">
-        <v>12</v>
+        <v>23</v>
       </c>
       <c r="Q25" s="48"/>
       <c r="R25" s="20"/>
@@ -2711,18 +2793,18 @@
         <f t="shared" si="0"/>
         <v>6</v>
       </c>
-      <c r="D26" s="59">
-        <v>0</v>
+      <c r="D26" s="82" t="s">
+        <v>13</v>
       </c>
       <c r="E26" s="60"/>
       <c r="F26" s="61"/>
-      <c r="G26" s="59">
-        <v>0</v>
+      <c r="G26" s="82" t="s">
+        <v>34</v>
       </c>
       <c r="H26" s="60"/>
       <c r="I26" s="61"/>
-      <c r="J26" s="59">
-        <v>0</v>
+      <c r="J26" s="82" t="s">
+        <v>15</v>
       </c>
       <c r="K26" s="60"/>
       <c r="L26" s="61"/>
@@ -2733,7 +2815,7 @@
       <c r="N26" s="60"/>
       <c r="O26" s="61"/>
       <c r="P26" s="48" t="s">
-        <v>12</v>
+        <v>23</v>
       </c>
       <c r="Q26" s="48"/>
       <c r="R26" s="20"/>
@@ -2749,28 +2831,22 @@
         <f t="shared" si="0"/>
         <v>7</v>
       </c>
-      <c r="D27" s="59" t="s">
-        <v>12</v>
-      </c>
+      <c r="D27" s="82"/>
       <c r="E27" s="60"/>
       <c r="F27" s="61"/>
-      <c r="G27" s="59" t="s">
-        <v>12</v>
-      </c>
+      <c r="G27" s="82"/>
       <c r="H27" s="60"/>
       <c r="I27" s="61"/>
-      <c r="J27" s="59" t="s">
-        <v>12</v>
-      </c>
+      <c r="J27" s="82"/>
       <c r="K27" s="60"/>
       <c r="L27" s="61"/>
       <c r="M27" s="59" t="s">
-        <v>12</v>
+        <v>23</v>
       </c>
       <c r="N27" s="60"/>
       <c r="O27" s="61"/>
       <c r="P27" s="48" t="s">
-        <v>12</v>
+        <v>23</v>
       </c>
       <c r="Q27" s="48"/>
       <c r="R27" s="20"/>
@@ -2786,23 +2862,17 @@
         <f t="shared" si="0"/>
         <v>1</v>
       </c>
-      <c r="D28" s="59" t="s">
-        <v>12</v>
-      </c>
+      <c r="D28" s="82"/>
       <c r="E28" s="60"/>
       <c r="F28" s="61"/>
-      <c r="G28" s="59" t="s">
-        <v>12</v>
-      </c>
+      <c r="G28" s="82"/>
       <c r="H28" s="60"/>
       <c r="I28" s="61"/>
-      <c r="J28" s="59" t="s">
-        <v>12</v>
-      </c>
+      <c r="J28" s="82"/>
       <c r="K28" s="60"/>
       <c r="L28" s="61"/>
       <c r="M28" s="59" t="s">
-        <v>12</v>
+        <v>23</v>
       </c>
       <c r="N28" s="60"/>
       <c r="O28" s="61"/>
@@ -2821,18 +2891,18 @@
         <f t="shared" si="0"/>
         <v>2</v>
       </c>
-      <c r="D29" s="59">
-        <v>0</v>
+      <c r="D29" s="82" t="s">
+        <v>20</v>
       </c>
       <c r="E29" s="60"/>
       <c r="F29" s="61"/>
-      <c r="G29" s="59">
-        <v>0</v>
+      <c r="G29" s="82" t="s">
+        <v>14</v>
       </c>
       <c r="H29" s="60"/>
       <c r="I29" s="61"/>
-      <c r="J29" s="59">
-        <v>0</v>
+      <c r="J29" s="82" t="s">
+        <v>22</v>
       </c>
       <c r="K29" s="60"/>
       <c r="L29" s="61"/>
@@ -2843,7 +2913,7 @@
       <c r="N29" s="60"/>
       <c r="O29" s="61"/>
       <c r="P29" s="48" t="s">
-        <v>12</v>
+        <v>23</v>
       </c>
       <c r="Q29" s="48"/>
       <c r="R29" s="20"/>
@@ -2859,18 +2929,18 @@
         <f t="shared" si="0"/>
         <v>3</v>
       </c>
-      <c r="D30" s="59">
-        <v>0</v>
+      <c r="D30" s="82" t="s">
+        <v>24</v>
       </c>
       <c r="E30" s="60"/>
       <c r="F30" s="61"/>
-      <c r="G30" s="59">
-        <v>0</v>
+      <c r="G30" s="82" t="s">
+        <v>35</v>
       </c>
       <c r="H30" s="60"/>
       <c r="I30" s="61"/>
-      <c r="J30" s="59">
-        <v>0</v>
+      <c r="J30" s="82" t="s">
+        <v>15</v>
       </c>
       <c r="K30" s="60"/>
       <c r="L30" s="61"/>
@@ -2881,7 +2951,7 @@
       <c r="N30" s="60"/>
       <c r="O30" s="61"/>
       <c r="P30" s="48" t="s">
-        <v>12</v>
+        <v>23</v>
       </c>
       <c r="Q30" s="48"/>
       <c r="R30" s="20"/>
@@ -2897,18 +2967,18 @@
         <f t="shared" si="0"/>
         <v>4</v>
       </c>
-      <c r="D31" s="59">
-        <v>0</v>
+      <c r="D31" s="82" t="s">
+        <v>24</v>
       </c>
       <c r="E31" s="60"/>
       <c r="F31" s="61"/>
-      <c r="G31" s="59">
-        <v>0</v>
+      <c r="G31" s="82" t="s">
+        <v>14</v>
       </c>
       <c r="H31" s="60"/>
       <c r="I31" s="61"/>
-      <c r="J31" s="59">
-        <v>0</v>
+      <c r="J31" s="82" t="s">
+        <v>31</v>
       </c>
       <c r="K31" s="60"/>
       <c r="L31" s="61"/>
@@ -2933,18 +3003,18 @@
         <f t="shared" si="0"/>
         <v>5</v>
       </c>
-      <c r="D32" s="59">
-        <v>0</v>
+      <c r="D32" s="82" t="s">
+        <v>17</v>
       </c>
       <c r="E32" s="60"/>
       <c r="F32" s="61"/>
-      <c r="G32" s="59">
-        <v>0</v>
+      <c r="G32" s="82" t="s">
+        <v>34</v>
       </c>
       <c r="H32" s="60"/>
       <c r="I32" s="61"/>
-      <c r="J32" s="59">
-        <v>0</v>
+      <c r="J32" s="82" t="s">
+        <v>15</v>
       </c>
       <c r="K32" s="60"/>
       <c r="L32" s="61"/>
@@ -2955,7 +3025,7 @@
       <c r="N32" s="60"/>
       <c r="O32" s="61"/>
       <c r="P32" s="48" t="s">
-        <v>12</v>
+        <v>23</v>
       </c>
       <c r="Q32" s="48"/>
       <c r="R32" s="20"/>
@@ -2971,18 +3041,18 @@
         <f t="shared" si="0"/>
         <v>6</v>
       </c>
-      <c r="D33" s="59">
-        <v>0</v>
+      <c r="D33" s="82" t="s">
+        <v>20</v>
       </c>
       <c r="E33" s="60"/>
       <c r="F33" s="61"/>
-      <c r="G33" s="59">
-        <v>0</v>
+      <c r="G33" s="82" t="s">
+        <v>14</v>
       </c>
       <c r="H33" s="60"/>
       <c r="I33" s="61"/>
-      <c r="J33" s="59">
-        <v>0</v>
+      <c r="J33" s="82" t="s">
+        <v>15</v>
       </c>
       <c r="K33" s="60"/>
       <c r="L33" s="61"/>
@@ -2993,7 +3063,7 @@
       <c r="N33" s="60"/>
       <c r="O33" s="61"/>
       <c r="P33" s="48" t="s">
-        <v>12</v>
+        <v>23</v>
       </c>
       <c r="Q33" s="48"/>
       <c r="R33" s="20"/>
@@ -3009,32 +3079,26 @@
         <f t="shared" si="0"/>
         <v>7</v>
       </c>
-      <c r="D34" s="59" t="s">
-        <v>12</v>
-      </c>
+      <c r="D34" s="82"/>
       <c r="E34" s="60"/>
       <c r="F34" s="61"/>
-      <c r="G34" s="59" t="s">
-        <v>12</v>
-      </c>
+      <c r="G34" s="82"/>
       <c r="H34" s="60"/>
       <c r="I34" s="61"/>
-      <c r="J34" s="59" t="s">
-        <v>12</v>
-      </c>
+      <c r="J34" s="82"/>
       <c r="K34" s="60"/>
       <c r="L34" s="61"/>
       <c r="M34" s="59" t="s">
-        <v>12</v>
+        <v>23</v>
       </c>
       <c r="N34" s="60"/>
       <c r="O34" s="61"/>
       <c r="P34" s="48" t="s">
-        <v>12</v>
+        <v>23</v>
       </c>
       <c r="Q34" s="48"/>
       <c r="R34" s="38" t="s">
-        <v>12</v>
+        <v>23</v>
       </c>
       <c r="S34" s="16"/>
       <c r="T34" s="17"/>
@@ -3048,30 +3112,24 @@
         <f t="shared" si="0"/>
         <v>1</v>
       </c>
-      <c r="D35" s="59" t="s">
-        <v>12</v>
-      </c>
+      <c r="D35" s="83"/>
       <c r="E35" s="60"/>
       <c r="F35" s="61"/>
-      <c r="G35" s="59" t="s">
-        <v>12</v>
-      </c>
+      <c r="G35" s="83"/>
       <c r="H35" s="60"/>
       <c r="I35" s="61"/>
-      <c r="J35" s="59" t="s">
-        <v>12</v>
-      </c>
+      <c r="J35" s="83"/>
       <c r="K35" s="60"/>
       <c r="L35" s="61"/>
       <c r="M35" s="59" t="s">
-        <v>12</v>
+        <v>23</v>
       </c>
       <c r="N35" s="60"/>
       <c r="O35" s="61"/>
       <c r="P35" s="48"/>
       <c r="Q35" s="48"/>
       <c r="R35" s="38" t="s">
-        <v>12</v>
+        <v>23</v>
       </c>
       <c r="S35" s="16"/>
       <c r="T35" s="17"/>
@@ -3085,18 +3143,18 @@
         <f t="shared" si="0"/>
         <v>2</v>
       </c>
-      <c r="D36" s="59">
-        <v>0</v>
+      <c r="D36" s="83" t="s">
+        <v>17</v>
       </c>
       <c r="E36" s="60"/>
       <c r="F36" s="61"/>
-      <c r="G36" s="59">
-        <v>0</v>
+      <c r="G36" s="83" t="s">
+        <v>34</v>
       </c>
       <c r="H36" s="60"/>
       <c r="I36" s="61"/>
-      <c r="J36" s="59">
-        <v>0</v>
+      <c r="J36" s="83" t="s">
+        <v>15</v>
       </c>
       <c r="K36" s="60"/>
       <c r="L36" s="61"/>
@@ -3107,11 +3165,11 @@
       <c r="N36" s="60"/>
       <c r="O36" s="61"/>
       <c r="P36" s="48" t="s">
-        <v>12</v>
+        <v>23</v>
       </c>
       <c r="Q36" s="48"/>
       <c r="R36" s="38" t="s">
-        <v>12</v>
+        <v>23</v>
       </c>
       <c r="S36" s="16"/>
       <c r="T36" s="17"/>
@@ -3125,18 +3183,18 @@
         <f t="shared" si="0"/>
         <v>3</v>
       </c>
-      <c r="D37" s="59">
-        <v>0</v>
+      <c r="D37" s="83" t="s">
+        <v>30</v>
       </c>
       <c r="E37" s="60"/>
       <c r="F37" s="61"/>
-      <c r="G37" s="59">
-        <v>0</v>
+      <c r="G37" s="83" t="s">
+        <v>36</v>
       </c>
       <c r="H37" s="60"/>
       <c r="I37" s="61"/>
-      <c r="J37" s="59">
-        <v>0</v>
+      <c r="J37" s="83" t="s">
+        <v>15</v>
       </c>
       <c r="K37" s="60"/>
       <c r="L37" s="61"/>
@@ -3149,42 +3207,42 @@
       <c r="P37" s="48"/>
       <c r="Q37" s="48"/>
       <c r="R37" s="38" t="s">
-        <v>12</v>
+        <v>23</v>
       </c>
       <c r="S37" s="16"/>
       <c r="T37" s="17"/>
     </row>
     <row r="38" ht="21.75" customHeight="1">
       <c r="B38" s="19" t="s">
-        <v>12</v>
+        <v>23</v>
       </c>
       <c r="C38" s="15" t="s">
-        <v>12</v>
+        <v>23</v>
       </c>
       <c r="D38" s="59" t="s">
-        <v>12</v>
+        <v>23</v>
       </c>
       <c r="E38" s="60"/>
       <c r="F38" s="61"/>
       <c r="G38" s="59" t="s">
-        <v>12</v>
+        <v>23</v>
       </c>
       <c r="H38" s="60"/>
       <c r="I38" s="61"/>
       <c r="J38" s="59" t="s">
-        <v>12</v>
+        <v>23</v>
       </c>
       <c r="K38" s="60"/>
       <c r="L38" s="61"/>
       <c r="M38" s="59" t="s">
-        <v>12</v>
+        <v>23</v>
       </c>
       <c r="N38" s="60"/>
       <c r="O38" s="61"/>
       <c r="P38" s="48"/>
       <c r="Q38" s="48"/>
       <c r="R38" s="38" t="s">
-        <v>12</v>
+        <v>23</v>
       </c>
       <c r="S38" s="16"/>
       <c r="T38" s="17"/>
@@ -3194,7 +3252,7 @@
       <c r="C39" s="24"/>
       <c r="D39" s="25"/>
       <c r="E39" s="40" t="s">
-        <v>13</v>
+        <v>37</v>
       </c>
       <c r="F39" s="25"/>
       <c r="G39" s="25"/>
@@ -3202,7 +3260,7 @@
       <c r="I39" s="25"/>
       <c r="J39" s="25"/>
       <c r="K39" s="26" t="s">
-        <v>14</v>
+        <v>38</v>
       </c>
       <c r="L39" s="25"/>
       <c r="M39" s="64">
@@ -3212,7 +3270,7 @@
       <c r="N39" s="64"/>
       <c r="O39" s="64"/>
       <c r="P39" s="37" t="s">
-        <v>12</v>
+        <v>23</v>
       </c>
       <c r="Q39" s="37"/>
       <c r="R39" s="27"/>
@@ -3291,7 +3349,7 @@
     </row>
     <row r="44" ht="27" customHeight="1" s="31" customFormat="1">
       <c r="B44" s="67" t="s">
-        <v>15</v>
+        <v>39</v>
       </c>
       <c r="C44" s="68"/>
       <c r="D44" s="70">
@@ -3300,7 +3358,7 @@
       <c r="E44" s="70"/>
       <c r="F44" s="70"/>
       <c r="G44" s="67" t="s">
-        <v>16</v>
+        <v>40</v>
       </c>
       <c r="H44" s="71"/>
       <c r="I44" s="68"/>
@@ -3312,7 +3370,7 @@
       <c r="L44" s="70"/>
       <c r="M44" s="73"/>
       <c r="N44" s="67" t="s">
-        <v>17</v>
+        <v>41</v>
       </c>
       <c r="O44" s="71"/>
       <c r="P44" s="62" t="str">
@@ -17132,21 +17190,12 @@
   </sheetData>
   <mergeCells>
     <mergeCell ref="M11:O11"/>
-    <mergeCell ref="J11:L11"/>
-    <mergeCell ref="G11:I11"/>
-    <mergeCell ref="D11:F11"/>
     <mergeCell ref="K48:L48"/>
     <mergeCell ref="D44:F44"/>
     <mergeCell ref="G44:I44"/>
     <mergeCell ref="J44:M44"/>
     <mergeCell ref="N44:O44"/>
-    <mergeCell ref="D36:F36"/>
-    <mergeCell ref="G36:I36"/>
-    <mergeCell ref="J36:L36"/>
     <mergeCell ref="M36:O36"/>
-    <mergeCell ref="D37:F37"/>
-    <mergeCell ref="G37:I37"/>
-    <mergeCell ref="J37:L37"/>
     <mergeCell ref="P44:Q44"/>
     <mergeCell ref="D38:F38"/>
     <mergeCell ref="G38:I38"/>
@@ -17156,121 +17205,130 @@
     <mergeCell ref="B42:R42"/>
     <mergeCell ref="B44:C44"/>
     <mergeCell ref="M37:O37"/>
+    <mergeCell ref="M34:O34"/>
+    <mergeCell ref="M35:O35"/>
+    <mergeCell ref="M32:O32"/>
+    <mergeCell ref="M33:O33"/>
+    <mergeCell ref="M30:O30"/>
+    <mergeCell ref="M31:O31"/>
+    <mergeCell ref="M28:O28"/>
+    <mergeCell ref="M29:O29"/>
+    <mergeCell ref="M26:O26"/>
+    <mergeCell ref="M27:O27"/>
+    <mergeCell ref="M24:O24"/>
+    <mergeCell ref="M25:O25"/>
+    <mergeCell ref="M22:O22"/>
+    <mergeCell ref="M23:O23"/>
+    <mergeCell ref="M20:O20"/>
+    <mergeCell ref="M21:O21"/>
+    <mergeCell ref="M18:O18"/>
+    <mergeCell ref="M19:O19"/>
+    <mergeCell ref="M16:O16"/>
+    <mergeCell ref="M17:O17"/>
+    <mergeCell ref="M14:O14"/>
+    <mergeCell ref="M15:O15"/>
+    <mergeCell ref="M12:O12"/>
+    <mergeCell ref="M13:O13"/>
+    <mergeCell ref="M10:O10"/>
+    <mergeCell ref="M7:O7"/>
+    <mergeCell ref="M8:O8"/>
+    <mergeCell ref="M9:O9"/>
+    <mergeCell ref="B3:E3"/>
+    <mergeCell ref="G3:J3"/>
+    <mergeCell ref="D7:F7"/>
+    <mergeCell ref="G7:I7"/>
+    <mergeCell ref="J7:L7"/>
+    <mergeCell ref="C5:I5"/>
+    <mergeCell ref="D8:F8"/>
+    <mergeCell ref="G8:I8"/>
+    <mergeCell ref="J8:L8"/>
+    <mergeCell ref="D9:F9"/>
+    <mergeCell ref="G9:I9"/>
+    <mergeCell ref="J9:L9"/>
+    <mergeCell ref="D10:F10"/>
+    <mergeCell ref="G10:I10"/>
+    <mergeCell ref="J10:L10"/>
+    <mergeCell ref="D11:F11"/>
+    <mergeCell ref="G11:I11"/>
+    <mergeCell ref="J11:L11"/>
+    <mergeCell ref="D12:F12"/>
+    <mergeCell ref="G12:I12"/>
+    <mergeCell ref="J12:L12"/>
+    <mergeCell ref="D13:F13"/>
+    <mergeCell ref="G13:I13"/>
+    <mergeCell ref="J13:L13"/>
+    <mergeCell ref="D14:F14"/>
+    <mergeCell ref="G14:I14"/>
+    <mergeCell ref="J14:L14"/>
+    <mergeCell ref="D15:F15"/>
+    <mergeCell ref="G15:I15"/>
+    <mergeCell ref="J15:L15"/>
+    <mergeCell ref="D16:F16"/>
+    <mergeCell ref="G16:I16"/>
+    <mergeCell ref="J16:L16"/>
+    <mergeCell ref="D17:F17"/>
+    <mergeCell ref="G17:I17"/>
+    <mergeCell ref="J17:L17"/>
+    <mergeCell ref="D18:F18"/>
+    <mergeCell ref="G18:I18"/>
+    <mergeCell ref="J18:L18"/>
+    <mergeCell ref="D19:F19"/>
+    <mergeCell ref="G19:I19"/>
+    <mergeCell ref="J19:L19"/>
+    <mergeCell ref="D20:F20"/>
+    <mergeCell ref="G20:I20"/>
+    <mergeCell ref="J20:L20"/>
+    <mergeCell ref="D21:F21"/>
+    <mergeCell ref="G21:I21"/>
+    <mergeCell ref="J21:L21"/>
+    <mergeCell ref="D22:F22"/>
+    <mergeCell ref="G22:I22"/>
+    <mergeCell ref="J22:L22"/>
+    <mergeCell ref="D23:F23"/>
+    <mergeCell ref="G23:I23"/>
+    <mergeCell ref="J23:L23"/>
+    <mergeCell ref="D24:F24"/>
+    <mergeCell ref="G24:I24"/>
+    <mergeCell ref="J24:L24"/>
+    <mergeCell ref="D25:F25"/>
+    <mergeCell ref="G25:I25"/>
+    <mergeCell ref="J25:L25"/>
+    <mergeCell ref="D26:F26"/>
+    <mergeCell ref="G26:I26"/>
+    <mergeCell ref="J26:L26"/>
+    <mergeCell ref="D27:F27"/>
+    <mergeCell ref="G27:I27"/>
+    <mergeCell ref="J27:L27"/>
+    <mergeCell ref="D28:F28"/>
+    <mergeCell ref="G28:I28"/>
+    <mergeCell ref="J28:L28"/>
+    <mergeCell ref="D29:F29"/>
+    <mergeCell ref="G29:I29"/>
+    <mergeCell ref="J29:L29"/>
+    <mergeCell ref="D30:F30"/>
+    <mergeCell ref="G30:I30"/>
+    <mergeCell ref="J30:L30"/>
+    <mergeCell ref="D31:F31"/>
+    <mergeCell ref="G31:I31"/>
+    <mergeCell ref="J31:L31"/>
+    <mergeCell ref="D32:F32"/>
+    <mergeCell ref="G32:I32"/>
+    <mergeCell ref="J32:L32"/>
+    <mergeCell ref="D33:F33"/>
+    <mergeCell ref="G33:I33"/>
+    <mergeCell ref="J33:L33"/>
     <mergeCell ref="D34:F34"/>
     <mergeCell ref="G34:I34"/>
     <mergeCell ref="J34:L34"/>
-    <mergeCell ref="M34:O34"/>
     <mergeCell ref="D35:F35"/>
     <mergeCell ref="G35:I35"/>
     <mergeCell ref="J35:L35"/>
-    <mergeCell ref="M35:O35"/>
-    <mergeCell ref="D32:F32"/>
-    <mergeCell ref="G32:I32"/>
-    <mergeCell ref="J32:L32"/>
-    <mergeCell ref="M32:O32"/>
-    <mergeCell ref="D33:F33"/>
-    <mergeCell ref="G33:I33"/>
-    <mergeCell ref="J33:L33"/>
-    <mergeCell ref="M33:O33"/>
-    <mergeCell ref="D30:F30"/>
-    <mergeCell ref="G30:I30"/>
-    <mergeCell ref="J30:L30"/>
-    <mergeCell ref="M30:O30"/>
-    <mergeCell ref="D31:F31"/>
-    <mergeCell ref="G31:I31"/>
-    <mergeCell ref="J31:L31"/>
-    <mergeCell ref="M31:O31"/>
-    <mergeCell ref="D28:F28"/>
-    <mergeCell ref="G28:I28"/>
-    <mergeCell ref="J28:L28"/>
-    <mergeCell ref="M28:O28"/>
-    <mergeCell ref="D29:F29"/>
-    <mergeCell ref="G29:I29"/>
-    <mergeCell ref="J29:L29"/>
-    <mergeCell ref="M29:O29"/>
-    <mergeCell ref="D26:F26"/>
-    <mergeCell ref="G26:I26"/>
-    <mergeCell ref="J26:L26"/>
-    <mergeCell ref="M26:O26"/>
-    <mergeCell ref="D27:F27"/>
-    <mergeCell ref="G27:I27"/>
-    <mergeCell ref="J27:L27"/>
-    <mergeCell ref="M27:O27"/>
-    <mergeCell ref="D24:F24"/>
-    <mergeCell ref="G24:I24"/>
-    <mergeCell ref="J24:L24"/>
-    <mergeCell ref="M24:O24"/>
-    <mergeCell ref="D25:F25"/>
-    <mergeCell ref="G25:I25"/>
-    <mergeCell ref="J25:L25"/>
-    <mergeCell ref="M25:O25"/>
-    <mergeCell ref="D22:F22"/>
-    <mergeCell ref="G22:I22"/>
-    <mergeCell ref="J22:L22"/>
-    <mergeCell ref="M22:O22"/>
-    <mergeCell ref="D23:F23"/>
-    <mergeCell ref="G23:I23"/>
-    <mergeCell ref="J23:L23"/>
-    <mergeCell ref="M23:O23"/>
-    <mergeCell ref="D20:F20"/>
-    <mergeCell ref="G20:I20"/>
-    <mergeCell ref="J20:L20"/>
-    <mergeCell ref="M20:O20"/>
-    <mergeCell ref="D21:F21"/>
-    <mergeCell ref="G21:I21"/>
-    <mergeCell ref="J21:L21"/>
-    <mergeCell ref="M21:O21"/>
-    <mergeCell ref="D18:F18"/>
-    <mergeCell ref="G18:I18"/>
-    <mergeCell ref="J18:L18"/>
-    <mergeCell ref="M18:O18"/>
-    <mergeCell ref="D19:F19"/>
-    <mergeCell ref="G19:I19"/>
-    <mergeCell ref="J19:L19"/>
-    <mergeCell ref="M19:O19"/>
-    <mergeCell ref="D16:F16"/>
-    <mergeCell ref="G16:I16"/>
-    <mergeCell ref="J16:L16"/>
-    <mergeCell ref="M16:O16"/>
-    <mergeCell ref="D17:F17"/>
-    <mergeCell ref="G17:I17"/>
-    <mergeCell ref="J17:L17"/>
-    <mergeCell ref="M17:O17"/>
-    <mergeCell ref="D14:F14"/>
-    <mergeCell ref="G14:I14"/>
-    <mergeCell ref="J14:L14"/>
-    <mergeCell ref="M14:O14"/>
-    <mergeCell ref="D15:F15"/>
-    <mergeCell ref="G15:I15"/>
-    <mergeCell ref="J15:L15"/>
-    <mergeCell ref="M15:O15"/>
-    <mergeCell ref="D12:F12"/>
-    <mergeCell ref="G12:I12"/>
-    <mergeCell ref="J12:L12"/>
-    <mergeCell ref="M12:O12"/>
-    <mergeCell ref="D13:F13"/>
-    <mergeCell ref="G13:I13"/>
-    <mergeCell ref="J13:L13"/>
-    <mergeCell ref="M13:O13"/>
-    <mergeCell ref="D10:F10"/>
-    <mergeCell ref="G10:I10"/>
-    <mergeCell ref="J10:L10"/>
-    <mergeCell ref="M10:O10"/>
-    <mergeCell ref="M7:O7"/>
-    <mergeCell ref="D8:F8"/>
-    <mergeCell ref="G8:I8"/>
-    <mergeCell ref="J8:L8"/>
-    <mergeCell ref="M8:O8"/>
-    <mergeCell ref="D9:F9"/>
-    <mergeCell ref="G9:I9"/>
-    <mergeCell ref="J9:L9"/>
-    <mergeCell ref="M9:O9"/>
-    <mergeCell ref="B3:E3"/>
-    <mergeCell ref="G3:J3"/>
-    <mergeCell ref="C5:I5"/>
-    <mergeCell ref="D7:F7"/>
-    <mergeCell ref="G7:I7"/>
-    <mergeCell ref="J7:L7"/>
+    <mergeCell ref="D36:F36"/>
+    <mergeCell ref="G36:I36"/>
+    <mergeCell ref="J36:L36"/>
+    <mergeCell ref="D37:F37"/>
+    <mergeCell ref="G37:I37"/>
+    <mergeCell ref="J37:L37"/>
   </mergeCells>
   <phoneticPr fontId="2"/>
   <printOptions horizontalCentered="1"/>
@@ -17379,39 +17437,39 @@
     </row>
     <row r="7" ht="16.5" customHeight="1">
       <c r="B7" s="11" t="s">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="C7" s="11" t="s">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="D7" s="56" t="s">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="E7" s="57"/>
       <c r="F7" s="58"/>
       <c r="G7" s="56" t="s">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="H7" s="57"/>
       <c r="I7" s="58"/>
       <c r="J7" s="56" t="s">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="K7" s="57"/>
       <c r="L7" s="58"/>
       <c r="M7" s="56" t="s">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="N7" s="57"/>
       <c r="O7" s="58"/>
       <c r="P7" s="35" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="Q7" s="35" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="R7" s="12" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="S7" s="13"/>
     </row>
@@ -17446,11 +17504,11 @@
       <c r="N8" s="75"/>
       <c r="O8" s="76"/>
       <c r="P8" s="47" t="s">
-        <v>12</v>
+        <v>23</v>
       </c>
       <c r="Q8" s="47"/>
       <c r="R8" s="46" t="s">
-        <v>12</v>
+        <v>23</v>
       </c>
       <c r="S8" s="16"/>
       <c r="T8" s="17"/>
@@ -17488,7 +17546,7 @@
       <c r="P9" s="48"/>
       <c r="Q9" s="48"/>
       <c r="R9" s="38" t="s">
-        <v>12</v>
+        <v>23</v>
       </c>
       <c r="S9" s="16"/>
       <c r="T9" s="17"/>
@@ -17526,7 +17584,7 @@
       <c r="P10" s="48"/>
       <c r="Q10" s="48"/>
       <c r="R10" s="50" t="s">
-        <v>12</v>
+        <v>23</v>
       </c>
       <c r="S10" s="16"/>
       <c r="T10" s="17"/>
@@ -17541,31 +17599,31 @@
         <v>7</v>
       </c>
       <c r="D11" s="59" t="s">
-        <v>18</v>
+        <v>42</v>
       </c>
       <c r="E11" s="60"/>
       <c r="F11" s="61"/>
       <c r="G11" s="59" t="s">
-        <v>18</v>
+        <v>42</v>
       </c>
       <c r="H11" s="60"/>
       <c r="I11" s="61"/>
       <c r="J11" s="59" t="s">
-        <v>18</v>
+        <v>42</v>
       </c>
       <c r="K11" s="60"/>
       <c r="L11" s="61"/>
       <c r="M11" s="59" t="s">
-        <v>18</v>
+        <v>42</v>
       </c>
       <c r="N11" s="60"/>
       <c r="O11" s="61"/>
       <c r="P11" s="48" t="s">
-        <v>12</v>
+        <v>23</v>
       </c>
       <c r="Q11" s="48"/>
       <c r="R11" s="38" t="s">
-        <v>12</v>
+        <v>23</v>
       </c>
       <c r="S11" s="16"/>
       <c r="T11" s="17"/>
@@ -17580,29 +17638,29 @@
         <v>1</v>
       </c>
       <c r="D12" s="59" t="s">
-        <v>12</v>
+        <v>23</v>
       </c>
       <c r="E12" s="60"/>
       <c r="F12" s="61"/>
       <c r="G12" s="59" t="s">
-        <v>12</v>
+        <v>23</v>
       </c>
       <c r="H12" s="60"/>
       <c r="I12" s="61"/>
       <c r="J12" s="59" t="s">
-        <v>12</v>
+        <v>23</v>
       </c>
       <c r="K12" s="60"/>
       <c r="L12" s="61"/>
       <c r="M12" s="59" t="s">
-        <v>12</v>
+        <v>23</v>
       </c>
       <c r="N12" s="60"/>
       <c r="O12" s="61"/>
       <c r="P12" s="48"/>
       <c r="Q12" s="48"/>
       <c r="R12" s="38" t="s">
-        <v>12</v>
+        <v>23</v>
       </c>
       <c r="S12" s="22"/>
       <c r="T12" s="17"/>
@@ -17710,7 +17768,7 @@
       <c r="N15" s="60"/>
       <c r="O15" s="61"/>
       <c r="P15" s="48" t="s">
-        <v>12</v>
+        <v>23</v>
       </c>
       <c r="Q15" s="48"/>
       <c r="R15" s="20"/>
@@ -17799,22 +17857,22 @@
         <v>7</v>
       </c>
       <c r="D18" s="59" t="s">
-        <v>18</v>
+        <v>42</v>
       </c>
       <c r="E18" s="60"/>
       <c r="F18" s="61"/>
       <c r="G18" s="59" t="s">
-        <v>18</v>
+        <v>42</v>
       </c>
       <c r="H18" s="60"/>
       <c r="I18" s="61"/>
       <c r="J18" s="59" t="s">
-        <v>18</v>
+        <v>42</v>
       </c>
       <c r="K18" s="60"/>
       <c r="L18" s="61"/>
       <c r="M18" s="59" t="s">
-        <v>18</v>
+        <v>42</v>
       </c>
       <c r="N18" s="60"/>
       <c r="O18" s="61"/>
@@ -17834,22 +17892,22 @@
         <v>1</v>
       </c>
       <c r="D19" s="59" t="s">
-        <v>12</v>
+        <v>23</v>
       </c>
       <c r="E19" s="60"/>
       <c r="F19" s="61"/>
       <c r="G19" s="59" t="s">
-        <v>12</v>
+        <v>23</v>
       </c>
       <c r="H19" s="60"/>
       <c r="I19" s="61"/>
       <c r="J19" s="59" t="s">
-        <v>12</v>
+        <v>23</v>
       </c>
       <c r="K19" s="60"/>
       <c r="L19" s="61"/>
       <c r="M19" s="59" t="s">
-        <v>12</v>
+        <v>23</v>
       </c>
       <c r="N19" s="60"/>
       <c r="O19" s="61"/>
@@ -17890,7 +17948,7 @@
       <c r="N20" s="60"/>
       <c r="O20" s="61"/>
       <c r="P20" s="49" t="s">
-        <v>18</v>
+        <v>42</v>
       </c>
       <c r="Q20" s="48"/>
       <c r="R20" s="38"/>
@@ -17930,7 +17988,7 @@
       <c r="P21" s="48"/>
       <c r="Q21" s="48"/>
       <c r="R21" s="38" t="s">
-        <v>12</v>
+        <v>23</v>
       </c>
       <c r="S21" s="16"/>
       <c r="T21" s="17"/>
@@ -18002,7 +18060,7 @@
       <c r="N23" s="60"/>
       <c r="O23" s="61"/>
       <c r="P23" s="49" t="s">
-        <v>18</v>
+        <v>42</v>
       </c>
       <c r="Q23" s="48"/>
       <c r="R23" s="20"/>
@@ -18042,7 +18100,7 @@
       <c r="P24" s="48"/>
       <c r="Q24" s="48"/>
       <c r="R24" s="38" t="s">
-        <v>12</v>
+        <v>23</v>
       </c>
       <c r="S24" s="16"/>
       <c r="T24" s="17"/>
@@ -18057,27 +18115,27 @@
         <v>7</v>
       </c>
       <c r="D25" s="59" t="s">
-        <v>18</v>
+        <v>42</v>
       </c>
       <c r="E25" s="60"/>
       <c r="F25" s="61"/>
       <c r="G25" s="59" t="s">
-        <v>18</v>
+        <v>42</v>
       </c>
       <c r="H25" s="60"/>
       <c r="I25" s="61"/>
       <c r="J25" s="59" t="s">
-        <v>18</v>
+        <v>42</v>
       </c>
       <c r="K25" s="60"/>
       <c r="L25" s="61"/>
       <c r="M25" s="59" t="s">
-        <v>18</v>
+        <v>42</v>
       </c>
       <c r="N25" s="60"/>
       <c r="O25" s="61"/>
       <c r="P25" s="48" t="s">
-        <v>12</v>
+        <v>23</v>
       </c>
       <c r="Q25" s="48"/>
       <c r="R25" s="20"/>
@@ -18094,22 +18152,22 @@
         <v>1</v>
       </c>
       <c r="D26" s="59" t="s">
-        <v>12</v>
+        <v>23</v>
       </c>
       <c r="E26" s="60"/>
       <c r="F26" s="61"/>
       <c r="G26" s="59" t="s">
-        <v>12</v>
+        <v>23</v>
       </c>
       <c r="H26" s="60"/>
       <c r="I26" s="61"/>
       <c r="J26" s="59" t="s">
-        <v>12</v>
+        <v>23</v>
       </c>
       <c r="K26" s="60"/>
       <c r="L26" s="61"/>
       <c r="M26" s="59" t="s">
-        <v>12</v>
+        <v>23</v>
       </c>
       <c r="N26" s="60"/>
       <c r="O26" s="61"/>
@@ -18237,22 +18295,22 @@
         <v>5</v>
       </c>
       <c r="D30" s="59" t="s">
-        <v>12</v>
+        <v>23</v>
       </c>
       <c r="E30" s="60"/>
       <c r="F30" s="61"/>
       <c r="G30" s="59" t="s">
-        <v>12</v>
+        <v>23</v>
       </c>
       <c r="H30" s="60"/>
       <c r="I30" s="61"/>
       <c r="J30" s="59" t="s">
-        <v>19</v>
+        <v>43</v>
       </c>
       <c r="K30" s="60"/>
       <c r="L30" s="61"/>
       <c r="M30" s="59" t="s">
-        <v>12</v>
+        <v>23</v>
       </c>
       <c r="N30" s="60"/>
       <c r="O30" s="61"/>
@@ -18272,22 +18330,22 @@
         <v>6</v>
       </c>
       <c r="D31" s="59" t="s">
-        <v>12</v>
+        <v>23</v>
       </c>
       <c r="E31" s="60"/>
       <c r="F31" s="61"/>
       <c r="G31" s="59" t="s">
-        <v>12</v>
+        <v>23</v>
       </c>
       <c r="H31" s="60"/>
       <c r="I31" s="61"/>
       <c r="J31" s="59" t="s">
-        <v>12</v>
+        <v>23</v>
       </c>
       <c r="K31" s="60"/>
       <c r="L31" s="61"/>
       <c r="M31" s="59" t="s">
-        <v>12</v>
+        <v>23</v>
       </c>
       <c r="N31" s="60"/>
       <c r="O31" s="61"/>
@@ -18307,27 +18365,27 @@
         <v>7</v>
       </c>
       <c r="D32" s="59" t="s">
-        <v>18</v>
+        <v>42</v>
       </c>
       <c r="E32" s="60"/>
       <c r="F32" s="61"/>
       <c r="G32" s="59" t="s">
-        <v>18</v>
+        <v>42</v>
       </c>
       <c r="H32" s="60"/>
       <c r="I32" s="61"/>
       <c r="J32" s="59" t="s">
-        <v>18</v>
+        <v>42</v>
       </c>
       <c r="K32" s="60"/>
       <c r="L32" s="61"/>
       <c r="M32" s="59" t="s">
-        <v>18</v>
+        <v>42</v>
       </c>
       <c r="N32" s="60"/>
       <c r="O32" s="61"/>
       <c r="P32" s="48" t="s">
-        <v>12</v>
+        <v>23</v>
       </c>
       <c r="Q32" s="48"/>
       <c r="R32" s="20"/>
@@ -18344,22 +18402,22 @@
         <v>1</v>
       </c>
       <c r="D33" s="59" t="s">
-        <v>12</v>
+        <v>23</v>
       </c>
       <c r="E33" s="60"/>
       <c r="F33" s="61"/>
       <c r="G33" s="59" t="s">
-        <v>12</v>
+        <v>23</v>
       </c>
       <c r="H33" s="60"/>
       <c r="I33" s="61"/>
       <c r="J33" s="59" t="s">
-        <v>12</v>
+        <v>23</v>
       </c>
       <c r="K33" s="60"/>
       <c r="L33" s="61"/>
       <c r="M33" s="59" t="s">
-        <v>12</v>
+        <v>23</v>
       </c>
       <c r="N33" s="60"/>
       <c r="O33" s="61"/>
@@ -18438,7 +18496,7 @@
       <c r="P35" s="48"/>
       <c r="Q35" s="48"/>
       <c r="R35" s="43" t="s">
-        <v>12</v>
+        <v>23</v>
       </c>
       <c r="S35" s="16"/>
       <c r="T35" s="17"/>
@@ -18474,7 +18532,7 @@
       <c r="N36" s="60"/>
       <c r="O36" s="61"/>
       <c r="P36" s="49" t="s">
-        <v>18</v>
+        <v>42</v>
       </c>
       <c r="Q36" s="48"/>
       <c r="R36" s="20"/>
@@ -18512,11 +18570,11 @@
       <c r="N37" s="60"/>
       <c r="O37" s="61"/>
       <c r="P37" s="49" t="s">
-        <v>18</v>
+        <v>42</v>
       </c>
       <c r="Q37" s="48"/>
       <c r="R37" s="38" t="s">
-        <v>12</v>
+        <v>23</v>
       </c>
       <c r="S37" s="16"/>
       <c r="T37" s="17"/>
@@ -18552,11 +18610,11 @@
       <c r="N38" s="60"/>
       <c r="O38" s="61"/>
       <c r="P38" s="49" t="s">
-        <v>18</v>
+        <v>42</v>
       </c>
       <c r="Q38" s="48"/>
       <c r="R38" s="38" t="s">
-        <v>12</v>
+        <v>23</v>
       </c>
       <c r="S38" s="16"/>
       <c r="T38" s="17"/>
@@ -18566,7 +18624,7 @@
       <c r="C39" s="24"/>
       <c r="D39" s="25"/>
       <c r="E39" s="40" t="s">
-        <v>20</v>
+        <v>44</v>
       </c>
       <c r="F39" s="25"/>
       <c r="G39" s="25"/>
@@ -18574,7 +18632,7 @@
       <c r="I39" s="25"/>
       <c r="J39" s="25"/>
       <c r="K39" s="26" t="s">
-        <v>14</v>
+        <v>38</v>
       </c>
       <c r="L39" s="25"/>
       <c r="M39" s="64">
@@ -18584,7 +18642,7 @@
       <c r="N39" s="64"/>
       <c r="O39" s="64"/>
       <c r="P39" s="37" t="s">
-        <v>12</v>
+        <v>23</v>
       </c>
       <c r="Q39" s="37"/>
       <c r="R39" s="27"/>
@@ -18663,7 +18721,7 @@
     </row>
     <row r="44" ht="27" customHeight="1" s="31" customFormat="1">
       <c r="B44" s="67" t="s">
-        <v>15</v>
+        <v>39</v>
       </c>
       <c r="C44" s="68"/>
       <c r="D44" s="70">
@@ -18672,7 +18730,7 @@
       <c r="E44" s="70"/>
       <c r="F44" s="70"/>
       <c r="G44" s="67" t="s">
-        <v>16</v>
+        <v>40</v>
       </c>
       <c r="H44" s="71"/>
       <c r="I44" s="68"/>
@@ -18684,7 +18742,7 @@
       <c r="L44" s="70"/>
       <c r="M44" s="73"/>
       <c r="N44" s="67" t="s">
-        <v>17</v>
+        <v>41</v>
       </c>
       <c r="O44" s="71"/>
       <c r="P44" s="62" t="str">
@@ -32753,39 +32811,39 @@
     </row>
     <row r="7" ht="16.5" customHeight="1">
       <c r="B7" s="11" t="s">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="C7" s="11" t="s">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="D7" s="56" t="s">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="E7" s="57"/>
       <c r="F7" s="58"/>
       <c r="G7" s="56" t="s">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="H7" s="57"/>
       <c r="I7" s="58"/>
       <c r="J7" s="56" t="s">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="K7" s="57"/>
       <c r="L7" s="58"/>
       <c r="M7" s="56" t="s">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="N7" s="57"/>
       <c r="O7" s="58"/>
       <c r="P7" s="35" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="Q7" s="35" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="R7" s="12" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="S7" s="13"/>
     </row>
@@ -32799,29 +32857,29 @@
         <v>7</v>
       </c>
       <c r="D8" s="59" t="s">
-        <v>18</v>
+        <v>42</v>
       </c>
       <c r="E8" s="60"/>
       <c r="F8" s="61"/>
       <c r="G8" s="59" t="s">
-        <v>18</v>
+        <v>42</v>
       </c>
       <c r="H8" s="60"/>
       <c r="I8" s="61"/>
       <c r="J8" s="59" t="s">
-        <v>18</v>
+        <v>42</v>
       </c>
       <c r="K8" s="60"/>
       <c r="L8" s="61"/>
       <c r="M8" s="59" t="s">
-        <v>18</v>
+        <v>42</v>
       </c>
       <c r="N8" s="60"/>
       <c r="O8" s="61"/>
       <c r="P8" s="47"/>
       <c r="Q8" s="47"/>
       <c r="R8" s="44" t="s">
-        <v>12</v>
+        <v>23</v>
       </c>
       <c r="S8" s="16"/>
       <c r="T8" s="17"/>
@@ -32838,29 +32896,29 @@
         <v>1</v>
       </c>
       <c r="D9" s="59" t="s">
-        <v>12</v>
+        <v>23</v>
       </c>
       <c r="E9" s="60"/>
       <c r="F9" s="61"/>
       <c r="G9" s="59" t="s">
-        <v>12</v>
+        <v>23</v>
       </c>
       <c r="H9" s="60"/>
       <c r="I9" s="61"/>
       <c r="J9" s="59" t="s">
-        <v>12</v>
+        <v>23</v>
       </c>
       <c r="K9" s="60"/>
       <c r="L9" s="61"/>
       <c r="M9" s="59" t="s">
-        <v>12</v>
+        <v>23</v>
       </c>
       <c r="N9" s="60"/>
       <c r="O9" s="61"/>
       <c r="P9" s="48"/>
       <c r="Q9" s="48"/>
       <c r="R9" s="43" t="s">
-        <v>12</v>
+        <v>23</v>
       </c>
       <c r="S9" s="16"/>
       <c r="T9" s="17"/>
@@ -32934,7 +32992,7 @@
       <c r="N11" s="60"/>
       <c r="O11" s="61"/>
       <c r="P11" s="48" t="s">
-        <v>12</v>
+        <v>23</v>
       </c>
       <c r="Q11" s="48"/>
       <c r="R11" s="20"/>
@@ -32973,7 +33031,7 @@
       <c r="N12" s="60"/>
       <c r="O12" s="61"/>
       <c r="P12" s="49" t="s">
-        <v>18</v>
+        <v>42</v>
       </c>
       <c r="Q12" s="48"/>
       <c r="R12" s="21"/>
@@ -33049,7 +33107,7 @@
       <c r="N14" s="60"/>
       <c r="O14" s="61"/>
       <c r="P14" s="48" t="s">
-        <v>12</v>
+        <v>23</v>
       </c>
       <c r="Q14" s="48"/>
       <c r="R14" s="20"/>
@@ -33067,31 +33125,31 @@
         <v>7</v>
       </c>
       <c r="D15" s="59" t="s">
-        <v>18</v>
+        <v>42</v>
       </c>
       <c r="E15" s="60"/>
       <c r="F15" s="61"/>
       <c r="G15" s="59" t="s">
-        <v>18</v>
+        <v>42</v>
       </c>
       <c r="H15" s="60"/>
       <c r="I15" s="61"/>
       <c r="J15" s="59" t="s">
-        <v>18</v>
+        <v>42</v>
       </c>
       <c r="K15" s="60"/>
       <c r="L15" s="61"/>
       <c r="M15" s="59" t="s">
-        <v>18</v>
+        <v>42</v>
       </c>
       <c r="N15" s="60"/>
       <c r="O15" s="61"/>
       <c r="P15" s="48" t="s">
-        <v>12</v>
+        <v>23</v>
       </c>
       <c r="Q15" s="48"/>
       <c r="R15" s="38" t="s">
-        <v>12</v>
+        <v>23</v>
       </c>
       <c r="S15" s="16"/>
       <c r="T15" s="17"/>
@@ -33107,29 +33165,29 @@
         <v>1</v>
       </c>
       <c r="D16" s="59" t="s">
-        <v>12</v>
+        <v>23</v>
       </c>
       <c r="E16" s="60"/>
       <c r="F16" s="61"/>
       <c r="G16" s="59" t="s">
-        <v>12</v>
+        <v>23</v>
       </c>
       <c r="H16" s="60"/>
       <c r="I16" s="61"/>
       <c r="J16" s="59" t="s">
-        <v>12</v>
+        <v>23</v>
       </c>
       <c r="K16" s="60"/>
       <c r="L16" s="61"/>
       <c r="M16" s="59" t="s">
-        <v>12</v>
+        <v>23</v>
       </c>
       <c r="N16" s="60"/>
       <c r="O16" s="61"/>
       <c r="P16" s="48"/>
       <c r="Q16" s="48"/>
       <c r="R16" s="38" t="s">
-        <v>12</v>
+        <v>23</v>
       </c>
       <c r="S16" s="16"/>
       <c r="T16" s="17"/>
@@ -33145,29 +33203,29 @@
         <v>2</v>
       </c>
       <c r="D17" s="59" t="s">
-        <v>12</v>
+        <v>23</v>
       </c>
       <c r="E17" s="60"/>
       <c r="F17" s="61"/>
       <c r="G17" s="59" t="s">
-        <v>12</v>
+        <v>23</v>
       </c>
       <c r="H17" s="60"/>
       <c r="I17" s="61"/>
       <c r="J17" s="59" t="s">
-        <v>12</v>
+        <v>23</v>
       </c>
       <c r="K17" s="60"/>
       <c r="L17" s="61"/>
       <c r="M17" s="59" t="s">
-        <v>12</v>
+        <v>23</v>
       </c>
       <c r="N17" s="60"/>
       <c r="O17" s="61"/>
       <c r="P17" s="48"/>
       <c r="Q17" s="48"/>
       <c r="R17" s="38" t="s">
-        <v>21</v>
+        <v>45</v>
       </c>
       <c r="S17" s="16"/>
       <c r="T17" s="17"/>
@@ -33183,33 +33241,33 @@
         <v>3</v>
       </c>
       <c r="D18" s="59" t="s">
-        <v>12</v>
+        <v>23</v>
       </c>
       <c r="E18" s="60"/>
       <c r="F18" s="61"/>
       <c r="G18" s="59" t="s">
-        <v>12</v>
+        <v>23</v>
       </c>
       <c r="H18" s="60"/>
       <c r="I18" s="61"/>
       <c r="J18" s="59" t="s">
-        <v>12</v>
+        <v>23</v>
       </c>
       <c r="K18" s="60"/>
       <c r="L18" s="61"/>
       <c r="M18" s="59" t="s">
-        <v>12</v>
+        <v>23</v>
       </c>
       <c r="N18" s="60"/>
       <c r="O18" s="61"/>
       <c r="P18" s="48" t="s">
-        <v>12</v>
+        <v>23</v>
       </c>
       <c r="Q18" s="48" t="s">
-        <v>12</v>
+        <v>23</v>
       </c>
       <c r="R18" s="38" t="s">
-        <v>21</v>
+        <v>45</v>
       </c>
       <c r="S18" s="16"/>
       <c r="T18" s="17"/>
@@ -33225,31 +33283,31 @@
         <v>4</v>
       </c>
       <c r="D19" s="59" t="s">
-        <v>12</v>
+        <v>23</v>
       </c>
       <c r="E19" s="60"/>
       <c r="F19" s="61"/>
       <c r="G19" s="59" t="s">
-        <v>12</v>
+        <v>23</v>
       </c>
       <c r="H19" s="60"/>
       <c r="I19" s="61"/>
       <c r="J19" s="59" t="s">
-        <v>12</v>
+        <v>23</v>
       </c>
       <c r="K19" s="60"/>
       <c r="L19" s="61"/>
       <c r="M19" s="59" t="s">
-        <v>12</v>
+        <v>23</v>
       </c>
       <c r="N19" s="60"/>
       <c r="O19" s="61"/>
       <c r="P19" s="48" t="s">
-        <v>12</v>
+        <v>23</v>
       </c>
       <c r="Q19" s="48"/>
       <c r="R19" s="38" t="s">
-        <v>21</v>
+        <v>45</v>
       </c>
       <c r="S19" s="16"/>
       <c r="T19" s="17"/>
@@ -33265,29 +33323,29 @@
         <v>5</v>
       </c>
       <c r="D20" s="59" t="s">
-        <v>12</v>
+        <v>23</v>
       </c>
       <c r="E20" s="60"/>
       <c r="F20" s="61"/>
       <c r="G20" s="59" t="s">
-        <v>12</v>
+        <v>23</v>
       </c>
       <c r="H20" s="60"/>
       <c r="I20" s="61"/>
       <c r="J20" s="59" t="s">
-        <v>12</v>
+        <v>23</v>
       </c>
       <c r="K20" s="60"/>
       <c r="L20" s="61"/>
       <c r="M20" s="59" t="s">
-        <v>12</v>
+        <v>23</v>
       </c>
       <c r="N20" s="60"/>
       <c r="O20" s="61"/>
       <c r="P20" s="48"/>
       <c r="Q20" s="48"/>
       <c r="R20" s="38" t="s">
-        <v>21</v>
+        <v>45</v>
       </c>
       <c r="S20" s="16"/>
       <c r="T20" s="17"/>
@@ -33303,29 +33361,29 @@
         <v>6</v>
       </c>
       <c r="D21" s="59" t="s">
-        <v>12</v>
+        <v>23</v>
       </c>
       <c r="E21" s="60"/>
       <c r="F21" s="61"/>
       <c r="G21" s="59" t="s">
-        <v>12</v>
+        <v>23</v>
       </c>
       <c r="H21" s="60"/>
       <c r="I21" s="61"/>
       <c r="J21" s="59" t="s">
-        <v>19</v>
+        <v>43</v>
       </c>
       <c r="K21" s="60"/>
       <c r="L21" s="61"/>
       <c r="M21" s="59" t="s">
-        <v>12</v>
+        <v>23</v>
       </c>
       <c r="N21" s="60"/>
       <c r="O21" s="61"/>
       <c r="P21" s="48"/>
       <c r="Q21" s="48"/>
       <c r="R21" s="38" t="s">
-        <v>21</v>
+        <v>45</v>
       </c>
       <c r="S21" s="16"/>
       <c r="T21" s="17"/>
@@ -33341,29 +33399,29 @@
         <v>7</v>
       </c>
       <c r="D22" s="59" t="s">
-        <v>12</v>
+        <v>23</v>
       </c>
       <c r="E22" s="60"/>
       <c r="F22" s="61"/>
       <c r="G22" s="59" t="s">
-        <v>12</v>
+        <v>23</v>
       </c>
       <c r="H22" s="60"/>
       <c r="I22" s="61"/>
       <c r="J22" s="59" t="s">
-        <v>12</v>
+        <v>23</v>
       </c>
       <c r="K22" s="60"/>
       <c r="L22" s="61"/>
       <c r="M22" s="59" t="s">
-        <v>12</v>
+        <v>23</v>
       </c>
       <c r="N22" s="60"/>
       <c r="O22" s="61"/>
       <c r="P22" s="48"/>
       <c r="Q22" s="48"/>
       <c r="R22" s="38" t="s">
-        <v>12</v>
+        <v>23</v>
       </c>
       <c r="S22" s="16"/>
       <c r="T22" s="17"/>
@@ -33379,32 +33437,32 @@
         <v>1</v>
       </c>
       <c r="D23" s="59" t="s">
-        <v>12</v>
+        <v>23</v>
       </c>
       <c r="E23" s="60"/>
       <c r="F23" s="61"/>
       <c r="G23" s="59" t="s">
-        <v>12</v>
+        <v>23</v>
       </c>
       <c r="H23" s="60"/>
       <c r="I23" s="61"/>
       <c r="J23" s="59" t="s">
-        <v>12</v>
+        <v>23</v>
       </c>
       <c r="K23" s="60"/>
       <c r="L23" s="61"/>
       <c r="M23" s="59" t="s">
-        <v>12</v>
+        <v>23</v>
       </c>
       <c r="N23" s="60"/>
       <c r="O23" s="61"/>
       <c r="P23" s="48"/>
       <c r="Q23" s="48"/>
       <c r="R23" s="38" t="s">
-        <v>12</v>
+        <v>23</v>
       </c>
       <c r="S23" s="16" t="s">
-        <v>12</v>
+        <v>23</v>
       </c>
       <c r="T23" s="17"/>
       <c r="U23" s="18"/>
@@ -33442,7 +33500,7 @@
       <c r="P24" s="48"/>
       <c r="Q24" s="48"/>
       <c r="R24" s="38" t="s">
-        <v>12</v>
+        <v>23</v>
       </c>
       <c r="S24" s="16"/>
       <c r="T24" s="17"/>
@@ -33479,11 +33537,11 @@
       <c r="N25" s="60"/>
       <c r="O25" s="61"/>
       <c r="P25" s="49" t="s">
-        <v>18</v>
+        <v>42</v>
       </c>
       <c r="Q25" s="48"/>
       <c r="R25" s="38" t="s">
-        <v>12</v>
+        <v>23</v>
       </c>
       <c r="S25" s="16"/>
       <c r="T25" s="17"/>
@@ -33520,11 +33578,11 @@
       <c r="N26" s="60"/>
       <c r="O26" s="61"/>
       <c r="P26" s="48" t="s">
-        <v>12</v>
+        <v>23</v>
       </c>
       <c r="Q26" s="48"/>
       <c r="R26" s="38" t="s">
-        <v>12</v>
+        <v>23</v>
       </c>
       <c r="S26" s="16"/>
       <c r="T26" s="17"/>
@@ -33598,7 +33656,7 @@
       <c r="N28" s="60"/>
       <c r="O28" s="61"/>
       <c r="P28" s="48" t="s">
-        <v>12</v>
+        <v>23</v>
       </c>
       <c r="Q28" s="48"/>
       <c r="R28" s="20"/>
@@ -33616,22 +33674,22 @@
         <v>7</v>
       </c>
       <c r="D29" s="59" t="s">
-        <v>18</v>
+        <v>42</v>
       </c>
       <c r="E29" s="60"/>
       <c r="F29" s="61"/>
       <c r="G29" s="59" t="s">
-        <v>18</v>
+        <v>42</v>
       </c>
       <c r="H29" s="60"/>
       <c r="I29" s="61"/>
       <c r="J29" s="59" t="s">
-        <v>18</v>
+        <v>42</v>
       </c>
       <c r="K29" s="60"/>
       <c r="L29" s="61"/>
       <c r="M29" s="59" t="s">
-        <v>18</v>
+        <v>42</v>
       </c>
       <c r="N29" s="60"/>
       <c r="O29" s="61"/>
@@ -33652,27 +33710,27 @@
         <v>1</v>
       </c>
       <c r="D30" s="59" t="s">
-        <v>12</v>
+        <v>23</v>
       </c>
       <c r="E30" s="60"/>
       <c r="F30" s="61"/>
       <c r="G30" s="59" t="s">
-        <v>12</v>
+        <v>23</v>
       </c>
       <c r="H30" s="60"/>
       <c r="I30" s="61"/>
       <c r="J30" s="59" t="s">
-        <v>12</v>
+        <v>23</v>
       </c>
       <c r="K30" s="60"/>
       <c r="L30" s="61"/>
       <c r="M30" s="59" t="s">
-        <v>12</v>
+        <v>23</v>
       </c>
       <c r="N30" s="60"/>
       <c r="O30" s="61"/>
       <c r="P30" s="48" t="s">
-        <v>12</v>
+        <v>23</v>
       </c>
       <c r="Q30" s="48"/>
       <c r="R30" s="20"/>
@@ -33785,7 +33843,7 @@
       <c r="N33" s="60"/>
       <c r="O33" s="61"/>
       <c r="P33" s="48" t="s">
-        <v>12</v>
+        <v>23</v>
       </c>
       <c r="Q33" s="48"/>
       <c r="R33" s="20"/>
@@ -33824,7 +33882,7 @@
       <c r="N34" s="60"/>
       <c r="O34" s="61"/>
       <c r="P34" s="48" t="s">
-        <v>12</v>
+        <v>23</v>
       </c>
       <c r="Q34" s="48"/>
       <c r="R34" s="20"/>
@@ -33879,27 +33937,27 @@
         <v>7</v>
       </c>
       <c r="D36" s="59" t="s">
-        <v>18</v>
+        <v>42</v>
       </c>
       <c r="E36" s="60"/>
       <c r="F36" s="61"/>
       <c r="G36" s="59" t="s">
-        <v>18</v>
+        <v>42</v>
       </c>
       <c r="H36" s="60"/>
       <c r="I36" s="61"/>
       <c r="J36" s="59" t="s">
-        <v>18</v>
+        <v>42</v>
       </c>
       <c r="K36" s="60"/>
       <c r="L36" s="61"/>
       <c r="M36" s="59" t="s">
-        <v>18</v>
+        <v>42</v>
       </c>
       <c r="N36" s="60"/>
       <c r="O36" s="61"/>
       <c r="P36" s="48" t="s">
-        <v>12</v>
+        <v>23</v>
       </c>
       <c r="Q36" s="48"/>
       <c r="R36" s="20"/>
@@ -33917,27 +33975,27 @@
         <v>1</v>
       </c>
       <c r="D37" s="59" t="s">
-        <v>18</v>
+        <v>42</v>
       </c>
       <c r="E37" s="60"/>
       <c r="F37" s="61"/>
       <c r="G37" s="59" t="s">
-        <v>18</v>
+        <v>42</v>
       </c>
       <c r="H37" s="60"/>
       <c r="I37" s="61"/>
       <c r="J37" s="59" t="s">
-        <v>18</v>
+        <v>42</v>
       </c>
       <c r="K37" s="60"/>
       <c r="L37" s="61"/>
       <c r="M37" s="59" t="s">
-        <v>18</v>
+        <v>42</v>
       </c>
       <c r="N37" s="60"/>
       <c r="O37" s="61"/>
       <c r="P37" s="49" t="s">
-        <v>18</v>
+        <v>42</v>
       </c>
       <c r="Q37" s="48"/>
       <c r="R37" s="20"/>
@@ -33987,7 +34045,7 @@
       <c r="C39" s="24"/>
       <c r="D39" s="25"/>
       <c r="E39" s="40" t="s">
-        <v>22</v>
+        <v>46</v>
       </c>
       <c r="F39" s="25"/>
       <c r="G39" s="25"/>
@@ -33995,7 +34053,7 @@
       <c r="I39" s="25"/>
       <c r="J39" s="25"/>
       <c r="K39" s="26" t="s">
-        <v>14</v>
+        <v>38</v>
       </c>
       <c r="L39" s="25"/>
       <c r="M39" s="64">
@@ -34005,7 +34063,7 @@
       <c r="N39" s="64"/>
       <c r="O39" s="64"/>
       <c r="P39" s="37" t="s">
-        <v>12</v>
+        <v>23</v>
       </c>
       <c r="Q39" s="37"/>
       <c r="R39" s="27"/>
@@ -34085,7 +34143,7 @@
     </row>
     <row r="44" ht="27" customHeight="1" s="31" customFormat="1">
       <c r="B44" s="67" t="s">
-        <v>15</v>
+        <v>39</v>
       </c>
       <c r="C44" s="68"/>
       <c r="D44" s="70">
@@ -34094,7 +34152,7 @@
       <c r="E44" s="70"/>
       <c r="F44" s="70"/>
       <c r="G44" s="67" t="s">
-        <v>16</v>
+        <v>40</v>
       </c>
       <c r="H44" s="71"/>
       <c r="I44" s="68"/>
@@ -34106,7 +34164,7 @@
       <c r="L44" s="70"/>
       <c r="M44" s="73"/>
       <c r="N44" s="67" t="s">
-        <v>17</v>
+        <v>41</v>
       </c>
       <c r="O44" s="71"/>
       <c r="P44" s="62" t="str">

</xml_diff>